<commit_message>
update database schema documentation
</commit_message>
<xml_diff>
--- a/Doc/db_schema.xlsx
+++ b/Doc/db_schema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\WebProjects\MentalMaths\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B14732-0CCE-4DF5-A093-D4EE9444C44E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18DC1CC-4A23-4051-838C-B1197F43BB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{E3C0760C-A047-42AC-9F87-43DD3A0ED6E4}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" activeTab="1" xr2:uid="{E3C0760C-A047-42AC-9F87-43DD3A0ED6E4}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -38,20 +38,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>Se</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>email</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>joined_on</t>
   </si>
   <si>
@@ -59,6 +50,30 @@
   </si>
   <si>
     <t>username</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>operations</t>
+  </si>
+  <si>
+    <t>['addition', 'subtraction', 'multiplication']</t>
+  </si>
+  <si>
+    <t>['division', 'rootExtraction']</t>
+  </si>
+  <si>
+    <t>addition_digits</t>
+  </si>
+  <si>
+    <t>subtraction_digits</t>
+  </si>
+  <si>
+    <t>multiplication_digits</t>
+  </si>
+  <si>
+    <t>highscore</t>
   </si>
 </sst>
 </file>
@@ -74,12 +89,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -94,8 +115,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,27 +434,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21AFF9D-A496-4A89-B633-71D0669BA4BB}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -442,15 +464,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEE54E01-DE04-4B79-9B80-4B244EE4B638}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -460,15 +487,46 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E0A12C8-4D6B-44C1-B2E2-F1428748A894}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="32.9296875" customWidth="1"/>
+    <col min="3" max="5" width="15.59765625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2">
         <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B3" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>